<commit_message>
running to update manuscript figures/tables
</commit_message>
<xml_diff>
--- a/Results_Table.xlsx
+++ b/Results_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Documents\poly-omics-risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F9DE52-E265-47AF-A0E9-B366309C2473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B01A2FF-5F3F-4C61-844C-F1076F607EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9446BBDD-3839-6B41-B466-D0C6B0D96A1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9446BBDD-3839-6B41-B466-D0C6B0D96A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,12 +64,6 @@
     <t>–</t>
   </si>
   <si>
-    <t>2.68 [1.09, 6.59], 0.03</t>
-  </si>
-  <si>
-    <t>0.74 [0.53, 0.94], 0.33</t>
-  </si>
-  <si>
     <t>AUC [95% CI] Standardized Score + age + sex, Nagelkerke’s R2</t>
   </si>
   <si>
@@ -91,18 +85,9 @@
     <t>9.28 [1.53, 56.13], 0.02</t>
   </si>
   <si>
-    <t>2.52 [0.97, 6.50], 0.06</t>
-  </si>
-  <si>
-    <t>0.76 [0.58, 0.95], 0.40</t>
-  </si>
-  <si>
     <t>2.89 [0.62, 13.52], 0.2</t>
   </si>
   <si>
-    <t>0.68 [0.46, 0.89], 0.19</t>
-  </si>
-  <si>
     <t>0.43 [0.19, 0.67], 0.08</t>
   </si>
   <si>
@@ -127,9 +112,6 @@
     <t>0.78 [0.59, 0.98], 0.32</t>
   </si>
   <si>
-    <t>0.67 [0.46, 0.89], 0.04</t>
-  </si>
-  <si>
     <t>5.94 [1.38, 25.55], 0.02</t>
   </si>
   <si>
@@ -140,6 +122,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 1.24 [0.50, 3.09], 0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.38 [0.15, 0.62], 0.04 </t>
+  </si>
+  <si>
+    <t>0.47 [0.25, 0.69], 0.01</t>
+  </si>
+  <si>
+    <t>0.80 [0.63, 0.98], 0.46</t>
+  </si>
+  <si>
+    <t>3.14 [1.10, 9.00], 0.03</t>
+  </si>
+  <si>
+    <t>3.13 [1.19, 8.26], 0.02</t>
+  </si>
+  <si>
+    <t>0.77 [0.58, 0.96], 0.37</t>
   </si>
 </sst>
 </file>
@@ -529,21 +529,21 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F6" sqref="A1:F6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.25" style="4" customWidth="1"/>
     <col min="3" max="3" width="24.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.796875" style="3"/>
+    <col min="4" max="4" width="23.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -561,98 +561,98 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>30</v>

</xml_diff>